<commit_message>
documentado la iteracion 4
</commit_message>
<xml_diff>
--- a/planilla burn down4.xlsx
+++ b/planilla burn down4.xlsx
@@ -219,22 +219,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>8</c:v>
@@ -243,13 +243,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -318,34 +318,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.4</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.8</c:v>
+                  <c:v>16.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.200000000000001</c:v>
+                  <c:v>14.699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.6000000000000014</c:v>
+                  <c:v>12.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0000000000000018</c:v>
+                  <c:v>10.499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.4000000000000021</c:v>
+                  <c:v>8.3999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.8000000000000025</c:v>
+                  <c:v>6.2999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2000000000000024</c:v>
+                  <c:v>4.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6000000000000023</c:v>
+                  <c:v>2.0999999999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -365,11 +365,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91447296"/>
-        <c:axId val="91448832"/>
+        <c:axId val="55672832"/>
+        <c:axId val="55674368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91447296"/>
+        <c:axId val="55672832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +378,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91448832"/>
+        <c:crossAx val="55674368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -386,7 +386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91448832"/>
+        <c:axId val="55674368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +416,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91447296"/>
+        <c:crossAx val="55672832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -763,7 +763,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,22 +814,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -838,17 +838,17 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <f>SUM(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2)</f>
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -856,43 +856,43 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <f>SUM(B3,- (B3 / 10))</f>
-        <v>14.4</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="D3">
         <f>SUM(C3,- (B3 / 10))</f>
-        <v>12.8</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="E3">
         <f>SUM(D3,- (B3 / 10))</f>
-        <v>11.200000000000001</v>
+        <v>14.699999999999998</v>
       </c>
       <c r="F3">
         <f>SUM(E3,- (B3 / 10))</f>
-        <v>9.6000000000000014</v>
+        <v>12.599999999999998</v>
       </c>
       <c r="G3">
         <f>SUM(F3,- (B3 / 10))</f>
-        <v>8.0000000000000018</v>
+        <v>10.499999999999998</v>
       </c>
       <c r="H3">
         <f>SUM(G3,- (B3 / 10))</f>
-        <v>6.4000000000000021</v>
+        <v>8.3999999999999986</v>
       </c>
       <c r="I3">
         <f>SUM(H3,- (B3 / 10))</f>
-        <v>4.8000000000000025</v>
+        <v>6.2999999999999989</v>
       </c>
       <c r="J3">
         <f>SUM(I3,- (B3 / 10))</f>
-        <v>3.2000000000000024</v>
+        <v>4.1999999999999993</v>
       </c>
       <c r="K3">
         <f>SUM(J3,- (B3 / 10))</f>
-        <v>1.6000000000000023</v>
+        <v>2.0999999999999992</v>
       </c>
       <c r="L3">
         <v>0</v>

</xml_diff>